<commit_message>
Added and updated mounted pipeline
</commit_message>
<xml_diff>
--- a/Person_B_and_trucks/on_trucks/Processed_Mounted/10 wheels/Strong-Tread Time-Domain Segments/Strong Tread Time Domain segment 600-POS-POS10.xlsx
+++ b/Person_B_and_trucks/on_trucks/Processed_Mounted/10 wheels/Strong-Tread Time-Domain Segments/Strong Tread Time Domain segment 600-POS-POS10.xlsx
@@ -19,7 +19,25 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="143">
+  <si>
+    <t>Signal_Value_8</t>
+  </si>
+  <si>
+    <t>Signal_Value_9</t>
+  </si>
+  <si>
+    <t>Signal_Value_10</t>
+  </si>
+  <si>
+    <t>Signal_Value_11</t>
+  </si>
+  <si>
+    <t>Signal_Value_12</t>
+  </si>
+  <si>
+    <t>Signal_Value_13</t>
+  </si>
   <si>
     <t>Signal_Value_14</t>
   </si>
@@ -345,6 +363,15 @@
     <t>Signal_Value_121</t>
   </si>
   <si>
+    <t>Signal_Value_122</t>
+  </si>
+  <si>
+    <t>Signal_Value_123</t>
+  </si>
+  <si>
+    <t>Signal_Value_124</t>
+  </si>
+  <si>
     <t>Segment_ID</t>
   </si>
   <si>
@@ -417,10 +444,7 @@
     <t>Tread</t>
   </si>
   <si>
-    <t>11R22.5</t>
-  </si>
-  <si>
-    <t>702ZE-i</t>
+    <t>275-80R22.5</t>
   </si>
   <si>
     <t>Empty</t>
@@ -781,15 +805,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:DE6"/>
+  <dimension ref="A1:DN6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:109">
+    <row r="1" spans="1:118">
       <c r="A1" s="1" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1115,10 +1139,37 @@
       <c r="DE1" s="1" t="s">
         <v>107</v>
       </c>
+      <c r="DF1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="DG1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="DH1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="DI1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="DJ1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="DK1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="DL1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="DM1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="DN1" s="1" t="s">
+        <v>116</v>
+      </c>
     </row>
-    <row r="2" spans="1:109">
+    <row r="2" spans="1:118">
       <c r="A2" s="1" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -1127,115 +1178,115 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>0.1233766198757316</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>0.0116280901391492</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>0.1131662245396726</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>0.07033388768609482</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>0.0009814880291004332</v>
       </c>
       <c r="I2">
-        <v>0.001927016889482189</v>
+        <v>0.002666414273327052</v>
       </c>
       <c r="J2">
-        <v>0.003045871335652075</v>
+        <v>0.01756200582879544</v>
       </c>
       <c r="K2">
-        <v>0.002963031102229157</v>
+        <v>0.1051242784223236</v>
       </c>
       <c r="L2">
-        <v>0.002239909998484269</v>
+        <v>0.07768184950998402</v>
       </c>
       <c r="M2">
-        <v>0.001589304814002865</v>
+        <v>0.003703789962175995</v>
       </c>
       <c r="N2">
-        <v>0</v>
+        <v>0.0002342436452776017</v>
       </c>
       <c r="O2">
-        <v>0.000354957196118153</v>
+        <v>0.06612030279669744</v>
       </c>
       <c r="P2">
-        <v>0.02062871311891452</v>
+        <v>0.03262776198357229</v>
       </c>
       <c r="Q2">
-        <v>0.01860453928926617</v>
+        <v>0.008456345987456114</v>
       </c>
       <c r="R2">
-        <v>0.006797743305882328</v>
+        <v>0.0261132173495744</v>
       </c>
       <c r="S2">
-        <v>0</v>
+        <v>0.1094433582145264</v>
       </c>
       <c r="T2">
-        <v>0.002186882739753753</v>
+        <v>0.0427107047320469</v>
       </c>
       <c r="U2">
-        <v>0</v>
+        <v>0.0003315869840040971</v>
       </c>
       <c r="V2">
-        <v>0.00100177528973675</v>
+        <v>0.00692020138231275</v>
       </c>
       <c r="W2">
-        <v>0.01463175617342547</v>
+        <v>0.0472009687016432</v>
       </c>
       <c r="X2">
-        <v>0.06184969910366404</v>
+        <v>0.05634023706479805</v>
       </c>
       <c r="Y2">
-        <v>0.1283415560710081</v>
+        <v>0.02502423177933359</v>
       </c>
       <c r="Z2">
-        <v>0.0301621230179566</v>
+        <v>0.009101679519828409</v>
       </c>
       <c r="AA2">
-        <v>0</v>
+        <v>0.007542767799968574</v>
       </c>
       <c r="AB2">
-        <v>0.04635486427322275</v>
+        <v>0.007252011990047977</v>
       </c>
       <c r="AC2">
-        <v>0.08398515077515156</v>
+        <v>0.0005361444451345929</v>
       </c>
       <c r="AD2">
-        <v>0.08737972758774544</v>
+        <v>4.676705062316281E-06</v>
       </c>
       <c r="AE2">
-        <v>0.03733234067190737</v>
+        <v>0.0008338542410400273</v>
       </c>
       <c r="AF2">
-        <v>0.003482268302171813</v>
+        <v>0.001792075725699642</v>
       </c>
       <c r="AG2">
-        <v>0.001226652255521381</v>
+        <v>0.0009345905800867547</v>
       </c>
       <c r="AH2">
-        <v>0.02961237643719288</v>
+        <v>0.01102738685292333</v>
       </c>
       <c r="AI2">
-        <v>0.07541467536426683</v>
+        <v>0.01322700325261089</v>
       </c>
       <c r="AJ2">
-        <v>0.1012042513521955</v>
+        <v>0</v>
       </c>
       <c r="AK2">
-        <v>0.1234199875287195</v>
+        <v>0</v>
       </c>
       <c r="AL2">
-        <v>0.08522106638912898</v>
+        <v>0</v>
       </c>
       <c r="AM2">
-        <v>0.01110798855980452</v>
+        <v>0</v>
       </c>
       <c r="AN2">
-        <v>0.01793377105739516</v>
+        <v>0</v>
       </c>
       <c r="AO2">
         <v>0</v>
@@ -1444,10 +1495,37 @@
       <c r="DE2">
         <v>0</v>
       </c>
+      <c r="DF2">
+        <v>0</v>
+      </c>
+      <c r="DG2">
+        <v>0</v>
+      </c>
+      <c r="DH2">
+        <v>0</v>
+      </c>
+      <c r="DI2">
+        <v>0</v>
+      </c>
+      <c r="DJ2">
+        <v>0</v>
+      </c>
+      <c r="DK2">
+        <v>0</v>
+      </c>
+      <c r="DL2">
+        <v>0</v>
+      </c>
+      <c r="DM2">
+        <v>0</v>
+      </c>
+      <c r="DN2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:109">
+    <row r="3" spans="1:118">
       <c r="A3" s="1" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -1654,129 +1732,156 @@
         <v>0</v>
       </c>
       <c r="BR3">
-        <v>0.01081915549833977</v>
+        <v>0</v>
       </c>
       <c r="BS3">
-        <v>0.03150545622760514</v>
+        <v>0</v>
       </c>
       <c r="BT3">
-        <v>0.0009412968027981551</v>
+        <v>0</v>
       </c>
       <c r="BU3">
-        <v>0.02957296923288156</v>
+        <v>0</v>
       </c>
       <c r="BV3">
-        <v>0.00365266276575015</v>
+        <v>0</v>
       </c>
       <c r="BW3">
-        <v>0.0226601053510329</v>
+        <v>0</v>
       </c>
       <c r="BX3">
-        <v>0.01049109177287256</v>
+        <v>0</v>
       </c>
       <c r="BY3">
-        <v>0.003861244010750907</v>
+        <v>0</v>
       </c>
       <c r="BZ3">
-        <v>0.005087323522888578</v>
+        <v>0</v>
       </c>
       <c r="CA3">
-        <v>0.05523471642786364</v>
+        <v>0</v>
       </c>
       <c r="CB3">
-        <v>0.09795373551844404</v>
+        <v>0</v>
       </c>
       <c r="CC3">
-        <v>0.03622643547424274</v>
+        <v>0</v>
       </c>
       <c r="CD3">
-        <v>0.001505063720628425</v>
+        <v>0</v>
       </c>
       <c r="CE3">
-        <v>0.04349959624524099</v>
+        <v>0</v>
       </c>
       <c r="CF3">
-        <v>0.09960816607978097</v>
+        <v>0</v>
       </c>
       <c r="CG3">
-        <v>0.07714617218526805</v>
+        <v>0</v>
       </c>
       <c r="CH3">
-        <v>0.01286114035444341</v>
+        <v>0</v>
       </c>
       <c r="CI3">
-        <v>0.003746536511726264</v>
+        <v>0.04910644800970281</v>
       </c>
       <c r="CJ3">
-        <v>0.02138990895394243</v>
+        <v>0.005777436778493363</v>
       </c>
       <c r="CK3">
-        <v>0.03646515815991912</v>
+        <v>0.2116961385448968</v>
       </c>
       <c r="CL3">
-        <v>0.0497822206268818</v>
+        <v>0.07402432330263407</v>
       </c>
       <c r="CM3">
-        <v>0.04312951959152882</v>
+        <v>0.003957856078239561</v>
       </c>
       <c r="CN3">
-        <v>0.02748531932894833</v>
+        <v>0.0033091478338602</v>
       </c>
       <c r="CO3">
-        <v>0.02712223027743649</v>
+        <v>0.1165888347395389</v>
       </c>
       <c r="CP3">
-        <v>0.01271539163802314</v>
+        <v>0.2166158914189258</v>
       </c>
       <c r="CQ3">
-        <v>0.003971574723309799</v>
+        <v>4.973720553741602E-05</v>
       </c>
       <c r="CR3">
-        <v>0.04406644838254328</v>
+        <v>0.03432548787718528</v>
       </c>
       <c r="CS3">
-        <v>0.05649874560035503</v>
+        <v>0.01806197616346386</v>
       </c>
       <c r="CT3">
-        <v>0.0490098159251617</v>
+        <v>0.001445150197964427</v>
       </c>
       <c r="CU3">
-        <v>0.04073269527633599</v>
+        <v>0.02645422337453373</v>
       </c>
       <c r="CV3">
-        <v>0.02984066659997842</v>
+        <v>0.004986067627597993</v>
       </c>
       <c r="CW3">
-        <v>0.01141743721307759</v>
+        <v>0.01788898233437319</v>
       </c>
       <c r="CX3">
-        <v>0</v>
+        <v>0.05595680687358075</v>
       </c>
       <c r="CY3">
-        <v>0</v>
+        <v>0.01466013052289046</v>
       </c>
       <c r="CZ3">
-        <v>0</v>
+        <v>0.00707378602384077</v>
       </c>
       <c r="DA3">
-        <v>0</v>
+        <v>0.0005276088164777434</v>
       </c>
       <c r="DB3">
-        <v>0</v>
+        <v>0.003457207789068778</v>
       </c>
       <c r="DC3">
-        <v>0</v>
+        <v>0.02020584524746969</v>
       </c>
       <c r="DD3">
-        <v>0</v>
+        <v>0.03799916754746491</v>
       </c>
       <c r="DE3">
-        <v>0</v>
+        <v>0.00348416613851049</v>
+      </c>
+      <c r="DF3">
+        <v>0.006991768602461282</v>
+      </c>
+      <c r="DG3">
+        <v>0.005375073267219991</v>
+      </c>
+      <c r="DH3">
+        <v>0.0006786616817606566</v>
+      </c>
+      <c r="DI3">
+        <v>0.01713463868148599</v>
+      </c>
+      <c r="DJ3">
+        <v>0.0004246510418636446</v>
+      </c>
+      <c r="DK3">
+        <v>0.01344467443747857</v>
+      </c>
+      <c r="DL3">
+        <v>0.007006094215466977</v>
+      </c>
+      <c r="DM3">
+        <v>0.01633816898806903</v>
+      </c>
+      <c r="DN3">
+        <v>0.004953848637942992</v>
       </c>
     </row>
-    <row r="4" spans="1:109">
+    <row r="4" spans="1:118">
       <c r="A4" s="1" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -2007,105 +2112,132 @@
         <v>0</v>
       </c>
       <c r="BZ4">
-        <v>0.01407148980537029</v>
+        <v>0</v>
       </c>
       <c r="CA4">
-        <v>0.06536103621921394</v>
+        <v>0</v>
       </c>
       <c r="CB4">
-        <v>0.01224919805474558</v>
+        <v>0</v>
       </c>
       <c r="CC4">
-        <v>0.05943431887634319</v>
+        <v>0</v>
       </c>
       <c r="CD4">
-        <v>0.002746110841918467</v>
+        <v>0</v>
       </c>
       <c r="CE4">
-        <v>0.05017983602059909</v>
+        <v>0</v>
       </c>
       <c r="CF4">
-        <v>0.02775815213704066</v>
+        <v>0</v>
       </c>
       <c r="CG4">
-        <v>0.009685652740756723</v>
+        <v>0.05918418727449985</v>
       </c>
       <c r="CH4">
-        <v>0.001265266715375315</v>
+        <v>0.03140715596598245</v>
       </c>
       <c r="CI4">
-        <v>0.07092582705032921</v>
+        <v>0.08849254055798796</v>
       </c>
       <c r="CJ4">
-        <v>0.0806348151036472</v>
+        <v>0.02419347546879224</v>
       </c>
       <c r="CK4">
-        <v>0.02068363370218751</v>
+        <v>2.344416704849378E-05</v>
       </c>
       <c r="CL4">
-        <v>0.006565016630446295</v>
+        <v>0.04428856632397206</v>
       </c>
       <c r="CM4">
-        <v>0.06019588470400685</v>
+        <v>0.09077531092159211</v>
       </c>
       <c r="CN4">
-        <v>0.0934913871743132</v>
+        <v>0.06824424512519564</v>
       </c>
       <c r="CO4">
-        <v>0.05332081977414471</v>
+        <v>0.004779618135528854</v>
       </c>
       <c r="CP4">
-        <v>0.003845212828971124</v>
+        <v>0.00884249003982134</v>
       </c>
       <c r="CQ4">
-        <v>0.005338731744526845</v>
+        <v>0.001025597846070026</v>
       </c>
       <c r="CR4">
-        <v>0.02187940748966275</v>
+        <v>0.1750442886568517</v>
       </c>
       <c r="CS4">
-        <v>0.03403459025886572</v>
+        <v>0.002570523097492589</v>
       </c>
       <c r="CT4">
-        <v>0.04402887899475206</v>
+        <v>0.02255153501268244</v>
       </c>
       <c r="CU4">
-        <v>0.04295964006295126</v>
+        <v>0.07502669277289596</v>
       </c>
       <c r="CV4">
-        <v>0.02559624428798722</v>
+        <v>0.09045722985728052</v>
       </c>
       <c r="CW4">
-        <v>0.01397837739216771</v>
+        <v>0.02265337802030552</v>
       </c>
       <c r="CX4">
-        <v>0.002198429891434594</v>
+        <v>0.0002185666988119184</v>
       </c>
       <c r="CY4">
-        <v>0.006931254807327772</v>
+        <v>0.02843649877223436</v>
       </c>
       <c r="CZ4">
-        <v>0.03668168597275428</v>
+        <v>0.1058218862651921</v>
       </c>
       <c r="DA4">
-        <v>0.04960307567730907</v>
+        <v>0.02281273121486461</v>
       </c>
       <c r="DB4">
-        <v>0.03812560495198635</v>
+        <v>0.0006473389198070192</v>
       </c>
       <c r="DC4">
-        <v>0.02513253866504957</v>
+        <v>0.001632478525147847</v>
       </c>
       <c r="DD4">
-        <v>0.01644062273228039</v>
+        <v>0.002030846493902564</v>
       </c>
       <c r="DE4">
-        <v>0.004657258691535208</v>
+        <v>0.008431545779823706</v>
+      </c>
+      <c r="DF4">
+        <v>0.002882408768592512</v>
+      </c>
+      <c r="DG4">
+        <v>0.0002033099306284116</v>
+      </c>
+      <c r="DH4">
+        <v>0.0003425258938413149</v>
+      </c>
+      <c r="DI4">
+        <v>4.380927758659116E-05</v>
+      </c>
+      <c r="DJ4">
+        <v>0.008191882908166134</v>
+      </c>
+      <c r="DK4">
+        <v>0.0004733014246914928</v>
+      </c>
+      <c r="DL4">
+        <v>0.008270589882709171</v>
+      </c>
+      <c r="DM4">
+        <v>0</v>
+      </c>
+      <c r="DN4">
+        <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:109">
+    <row r="5" spans="1:118">
       <c r="A5" s="1" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -2219,100 +2351,100 @@
         <v>0</v>
       </c>
       <c r="AM5">
-        <v>0.04942376589392553</v>
+        <v>0</v>
       </c>
       <c r="AN5">
-        <v>0.01845631529732133</v>
+        <v>0</v>
       </c>
       <c r="AO5">
         <v>0</v>
       </c>
       <c r="AP5">
-        <v>0.006335992259331715</v>
+        <v>0</v>
       </c>
       <c r="AQ5">
-        <v>0.003844927094696123</v>
+        <v>0</v>
       </c>
       <c r="AR5">
-        <v>6.895801604571795E-05</v>
+        <v>0</v>
       </c>
       <c r="AS5">
-        <v>0.002452032279250784</v>
+        <v>0</v>
       </c>
       <c r="AT5">
-        <v>0.02303896288708042</v>
+        <v>0</v>
       </c>
       <c r="AU5">
-        <v>0.07059768002574465</v>
+        <v>0</v>
       </c>
       <c r="AV5">
-        <v>0.08839610671112183</v>
+        <v>0</v>
       </c>
       <c r="AW5">
-        <v>0.09348227198458259</v>
+        <v>0</v>
       </c>
       <c r="AX5">
-        <v>0.06240451345060934</v>
+        <v>0</v>
       </c>
       <c r="AY5">
-        <v>0.0435935645654829</v>
+        <v>0</v>
       </c>
       <c r="AZ5">
-        <v>0.01886526760884249</v>
+        <v>0</v>
       </c>
       <c r="BA5">
-        <v>0.02227583595496616</v>
+        <v>0</v>
       </c>
       <c r="BB5">
-        <v>0.02161027850702581</v>
+        <v>0</v>
       </c>
       <c r="BC5">
-        <v>0.001753308518394393</v>
+        <v>0</v>
       </c>
       <c r="BD5">
         <v>0</v>
       </c>
       <c r="BE5">
-        <v>0.002504411670465047</v>
+        <v>0</v>
       </c>
       <c r="BF5">
-        <v>0.0003484665532198532</v>
+        <v>0</v>
       </c>
       <c r="BG5">
         <v>0</v>
       </c>
       <c r="BH5">
-        <v>0.005443745538711343</v>
+        <v>0</v>
       </c>
       <c r="BI5">
-        <v>0.05086943216265886</v>
+        <v>0</v>
       </c>
       <c r="BJ5">
-        <v>0.08433772147130773</v>
+        <v>0</v>
       </c>
       <c r="BK5">
-        <v>0.08408873557757829</v>
+        <v>0</v>
       </c>
       <c r="BL5">
-        <v>0.03052599308047416</v>
+        <v>0</v>
       </c>
       <c r="BM5">
-        <v>0.01492087365320427</v>
+        <v>0</v>
       </c>
       <c r="BN5">
-        <v>0.0287382063178142</v>
+        <v>0</v>
       </c>
       <c r="BO5">
-        <v>0.06782646716092046</v>
+        <v>0</v>
       </c>
       <c r="BP5">
-        <v>0.06188353118362393</v>
+        <v>0</v>
       </c>
       <c r="BQ5">
         <v>0</v>
       </c>
       <c r="BR5">
-        <v>0.04191263457560022</v>
+        <v>0</v>
       </c>
       <c r="BS5">
         <v>0</v>
@@ -2354,87 +2486,114 @@
         <v>0</v>
       </c>
       <c r="CF5">
-        <v>0</v>
+        <v>0.03059814523646267</v>
       </c>
       <c r="CG5">
-        <v>0</v>
+        <v>0.01691277493205944</v>
       </c>
       <c r="CH5">
-        <v>0</v>
+        <v>0.04076431413764888</v>
       </c>
       <c r="CI5">
-        <v>0</v>
+        <v>0.009094867728524766</v>
       </c>
       <c r="CJ5">
-        <v>0</v>
+        <v>0.007044782690484351</v>
       </c>
       <c r="CK5">
-        <v>0</v>
+        <v>0.005907561793139656</v>
       </c>
       <c r="CL5">
-        <v>0</v>
+        <v>0.03646213055451533</v>
       </c>
       <c r="CM5">
-        <v>0</v>
+        <v>0.08781073225536434</v>
       </c>
       <c r="CN5">
-        <v>0</v>
+        <v>0.0001620104165293333</v>
       </c>
       <c r="CO5">
-        <v>0</v>
+        <v>0.03047068176241538</v>
       </c>
       <c r="CP5">
-        <v>0</v>
+        <v>0.02661253819755233</v>
       </c>
       <c r="CQ5">
-        <v>0</v>
+        <v>0.09928216601215256</v>
       </c>
       <c r="CR5">
-        <v>0</v>
+        <v>0.11108138231814</v>
       </c>
       <c r="CS5">
-        <v>0</v>
+        <v>0.01432613958257463</v>
       </c>
       <c r="CT5">
         <v>0</v>
       </c>
       <c r="CU5">
-        <v>0</v>
+        <v>0.1085268936776565</v>
       </c>
       <c r="CV5">
-        <v>0</v>
+        <v>0.0728822376790887</v>
       </c>
       <c r="CW5">
-        <v>0</v>
+        <v>0.0002334302240836762</v>
       </c>
       <c r="CX5">
         <v>0</v>
       </c>
       <c r="CY5">
-        <v>0</v>
+        <v>0.1190487193060183</v>
       </c>
       <c r="CZ5">
-        <v>0</v>
+        <v>0.1292104118804263</v>
       </c>
       <c r="DA5">
-        <v>0</v>
+        <v>0.001066980840762719</v>
       </c>
       <c r="DB5">
-        <v>0</v>
+        <v>0.006420918877577341</v>
       </c>
       <c r="DC5">
-        <v>0</v>
+        <v>0.001289928065346659</v>
       </c>
       <c r="DD5">
-        <v>0</v>
+        <v>0.002911812543949023</v>
       </c>
       <c r="DE5">
+        <v>0.001277234820819133</v>
+      </c>
+      <c r="DF5">
+        <v>0.009542734302018345</v>
+      </c>
+      <c r="DG5">
+        <v>0.002070135613025703</v>
+      </c>
+      <c r="DH5">
+        <v>0.0007971496575186148</v>
+      </c>
+      <c r="DI5">
+        <v>0.02324077887971839</v>
+      </c>
+      <c r="DJ5">
+        <v>0.004458009267995895</v>
+      </c>
+      <c r="DK5">
+        <v>0.0004923967464313614</v>
+      </c>
+      <c r="DL5">
+        <v>0</v>
+      </c>
+      <c r="DM5">
+        <v>0</v>
+      </c>
+      <c r="DN5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:109">
+    <row r="6" spans="1:118">
       <c r="A6" s="1" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -2443,100 +2602,100 @@
         <v>0</v>
       </c>
       <c r="D6">
-        <v>0.004111641918218757</v>
+        <v>0</v>
       </c>
       <c r="E6">
-        <v>0.0001254374029193167</v>
+        <v>0</v>
       </c>
       <c r="F6">
-        <v>0.006906231150942368</v>
+        <v>0</v>
       </c>
       <c r="G6">
-        <v>9.610466440191057E-07</v>
+        <v>0</v>
       </c>
       <c r="H6">
-        <v>0.002553432436902071</v>
+        <v>0</v>
       </c>
       <c r="I6">
-        <v>0.004311970762538047</v>
+        <v>0</v>
       </c>
       <c r="J6">
-        <v>0.0006423029875447074</v>
+        <v>0</v>
       </c>
       <c r="K6">
-        <v>0.00114094032970275</v>
+        <v>0</v>
       </c>
       <c r="L6">
-        <v>0.006366585042166835</v>
+        <v>0</v>
       </c>
       <c r="M6">
-        <v>0.01709410211291237</v>
+        <v>0</v>
       </c>
       <c r="N6">
-        <v>0.007344714816336877</v>
+        <v>0</v>
       </c>
       <c r="O6">
-        <v>9.859108399509448E-07</v>
+        <v>0</v>
       </c>
       <c r="P6">
-        <v>0.007278981787082524</v>
+        <v>0</v>
       </c>
       <c r="Q6">
-        <v>0.0171314323583025</v>
+        <v>0</v>
       </c>
       <c r="R6">
-        <v>0.01682241780435466</v>
+        <v>0</v>
       </c>
       <c r="S6">
-        <v>0.003932586440135471</v>
+        <v>0</v>
       </c>
       <c r="T6">
-        <v>8.137647911826533E-05</v>
+        <v>0</v>
       </c>
       <c r="U6">
-        <v>0.002615480160284464</v>
+        <v>0</v>
       </c>
       <c r="V6">
-        <v>0.005389005389596838</v>
+        <v>0</v>
       </c>
       <c r="W6">
-        <v>0.009743263084920708</v>
+        <v>0</v>
       </c>
       <c r="X6">
-        <v>0.04535279821810814</v>
+        <v>0</v>
       </c>
       <c r="Y6">
-        <v>0.0894686889482</v>
+        <v>0</v>
       </c>
       <c r="Z6">
-        <v>0.06957158787029667</v>
+        <v>0</v>
       </c>
       <c r="AA6">
-        <v>0.03122624656986156</v>
+        <v>0</v>
       </c>
       <c r="AB6">
-        <v>0.002883033016048734</v>
+        <v>0</v>
       </c>
       <c r="AC6">
-        <v>0.09386306933555595</v>
+        <v>0</v>
       </c>
       <c r="AD6">
-        <v>0.1602215240911982</v>
+        <v>0</v>
       </c>
       <c r="AE6">
-        <v>0.1426068396509511</v>
+        <v>0</v>
       </c>
       <c r="AF6">
-        <v>0.110779387691141</v>
+        <v>0</v>
       </c>
       <c r="AG6">
-        <v>0.09265596232906771</v>
+        <v>0</v>
       </c>
       <c r="AH6">
-        <v>0.0410245285385562</v>
+        <v>0</v>
       </c>
       <c r="AI6">
-        <v>0.006752484319551244</v>
+        <v>0</v>
       </c>
       <c r="AJ6">
         <v>0</v>
@@ -2686,78 +2845,105 @@
         <v>0</v>
       </c>
       <c r="CG6">
-        <v>0</v>
+        <v>0.05794142923749691</v>
       </c>
       <c r="CH6">
-        <v>0</v>
+        <v>0.007418025580896794</v>
       </c>
       <c r="CI6">
-        <v>0</v>
+        <v>0.09938309892083111</v>
       </c>
       <c r="CJ6">
-        <v>0</v>
+        <v>0.08405343678640025</v>
       </c>
       <c r="CK6">
-        <v>0</v>
+        <v>0.003613390765944549</v>
       </c>
       <c r="CL6">
-        <v>0</v>
+        <v>0.03837661341701729</v>
       </c>
       <c r="CM6">
-        <v>0</v>
+        <v>0.0562596152980397</v>
       </c>
       <c r="CN6">
-        <v>0</v>
+        <v>0.05934431250583446</v>
       </c>
       <c r="CO6">
-        <v>0</v>
+        <v>0.02177096689019573</v>
       </c>
       <c r="CP6">
-        <v>0</v>
+        <v>0.01253808375608249</v>
       </c>
       <c r="CQ6">
-        <v>0</v>
+        <v>8.636445370245564E-06</v>
       </c>
       <c r="CR6">
-        <v>0</v>
+        <v>0.1557357489422946</v>
       </c>
       <c r="CS6">
-        <v>0</v>
+        <v>0.007701137478443377</v>
       </c>
       <c r="CT6">
-        <v>0</v>
+        <v>0.03727943185200393</v>
       </c>
       <c r="CU6">
-        <v>0</v>
+        <v>0.00305046473457711</v>
       </c>
       <c r="CV6">
-        <v>0</v>
+        <v>0.09773996391449713</v>
       </c>
       <c r="CW6">
-        <v>0</v>
+        <v>0.082221987128529</v>
       </c>
       <c r="CX6">
-        <v>0</v>
+        <v>1.104332311288531E-05</v>
       </c>
       <c r="CY6">
-        <v>0</v>
+        <v>0.06191557209010418</v>
       </c>
       <c r="CZ6">
-        <v>0</v>
+        <v>0.08004007241457571</v>
       </c>
       <c r="DA6">
-        <v>0</v>
+        <v>1.169604797119121E-05</v>
       </c>
       <c r="DB6">
-        <v>0</v>
+        <v>0.0008421511983379165</v>
       </c>
       <c r="DC6">
-        <v>0</v>
+        <v>0.0002784023827904771</v>
       </c>
       <c r="DD6">
-        <v>0</v>
+        <v>0.004899943368627127</v>
       </c>
       <c r="DE6">
+        <v>0.001321454627140262</v>
+      </c>
+      <c r="DF6">
+        <v>0.005877114623054678</v>
+      </c>
+      <c r="DG6">
+        <v>0.00276860844752218</v>
+      </c>
+      <c r="DH6">
+        <v>0.0004427300900674052</v>
+      </c>
+      <c r="DI6">
+        <v>8.093604343584218E-05</v>
+      </c>
+      <c r="DJ6">
+        <v>0.007689978429172016</v>
+      </c>
+      <c r="DK6">
+        <v>5.332039520931474E-05</v>
+      </c>
+      <c r="DL6">
+        <v>0.009330632864424176</v>
+      </c>
+      <c r="DM6">
+        <v>0</v>
+      </c>
+      <c r="DN6">
         <v>0</v>
       </c>
     </row>
@@ -2768,15 +2954,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:DE6"/>
+  <dimension ref="A1:DN6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:109">
+    <row r="1" spans="1:118">
       <c r="A1" s="1" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -3102,10 +3288,37 @@
       <c r="DE1" s="1" t="s">
         <v>107</v>
       </c>
+      <c r="DF1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="DG1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="DH1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="DI1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="DJ1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="DK1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="DL1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="DM1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="DN1" s="1" t="s">
+        <v>116</v>
+      </c>
     </row>
-    <row r="2" spans="1:109">
+    <row r="2" spans="1:118">
       <c r="A2" s="1" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -3114,112 +3327,112 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>0.1233766198757316</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>0.1350047100148808</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>0.2481709345545534</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>0.3185048222406482</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>0.3194863102697486</v>
       </c>
       <c r="I2">
-        <v>0.001927016889482189</v>
+        <v>0.3221527245430756</v>
       </c>
       <c r="J2">
-        <v>0.004972888225134264</v>
+        <v>0.3397147303718711</v>
       </c>
       <c r="K2">
-        <v>0.007935919327363421</v>
+        <v>0.4448390087941947</v>
       </c>
       <c r="L2">
-        <v>0.01017582932584769</v>
+        <v>0.5225208583041787</v>
       </c>
       <c r="M2">
-        <v>0.01176513413985055</v>
+        <v>0.5262246482663547</v>
       </c>
       <c r="N2">
-        <v>0.01176513413985055</v>
+        <v>0.5264588919116323</v>
       </c>
       <c r="O2">
-        <v>0.01212009133596871</v>
+        <v>0.5925791947083298</v>
       </c>
       <c r="P2">
-        <v>0.03274880445488322</v>
+        <v>0.6252069566919021</v>
       </c>
       <c r="Q2">
-        <v>0.05135334374414939</v>
+        <v>0.6336633026793582</v>
       </c>
       <c r="R2">
-        <v>0.05815108705003172</v>
+        <v>0.6597765200289326</v>
       </c>
       <c r="S2">
-        <v>0.05815108705003172</v>
+        <v>0.7692198782434589</v>
       </c>
       <c r="T2">
-        <v>0.06033796978978547</v>
+        <v>0.8119305829755058</v>
       </c>
       <c r="U2">
-        <v>0.06033796978978547</v>
+        <v>0.8122621699595099</v>
       </c>
       <c r="V2">
-        <v>0.06133974507952222</v>
+        <v>0.8191823713418227</v>
       </c>
       <c r="W2">
-        <v>0.07597150125294769</v>
+        <v>0.866383340043466</v>
       </c>
       <c r="X2">
-        <v>0.1378212003566117</v>
+        <v>0.922723577108264</v>
       </c>
       <c r="Y2">
-        <v>0.2661627564276198</v>
+        <v>0.9477478088875976</v>
       </c>
       <c r="Z2">
-        <v>0.2963248794455764</v>
+        <v>0.956849488407426</v>
       </c>
       <c r="AA2">
-        <v>0.2963248794455764</v>
+        <v>0.9643922562073945</v>
       </c>
       <c r="AB2">
-        <v>0.3426797437187992</v>
+        <v>0.9716442681974425</v>
       </c>
       <c r="AC2">
-        <v>0.4266648944939507</v>
+        <v>0.9721804126425772</v>
       </c>
       <c r="AD2">
-        <v>0.5140446220816962</v>
+        <v>0.9721850893476395</v>
       </c>
       <c r="AE2">
-        <v>0.5513769627536036</v>
+        <v>0.9730189435886795</v>
       </c>
       <c r="AF2">
-        <v>0.5548592310557754</v>
+        <v>0.9748110193143791</v>
       </c>
       <c r="AG2">
-        <v>0.5560858833112968</v>
+        <v>0.9757456098944658</v>
       </c>
       <c r="AH2">
-        <v>0.5856982597484897</v>
+        <v>0.9867729967473892</v>
       </c>
       <c r="AI2">
-        <v>0.6611129351127565</v>
+        <v>1</v>
       </c>
       <c r="AJ2">
-        <v>0.7623171864649519</v>
+        <v>1</v>
       </c>
       <c r="AK2">
-        <v>0.8857371739936715</v>
+        <v>1</v>
       </c>
       <c r="AL2">
-        <v>0.9709582403828004</v>
+        <v>1</v>
       </c>
       <c r="AM2">
-        <v>0.982066228942605</v>
+        <v>1</v>
       </c>
       <c r="AN2">
         <v>1</v>
@@ -3431,10 +3644,37 @@
       <c r="DE2">
         <v>1</v>
       </c>
+      <c r="DF2">
+        <v>1</v>
+      </c>
+      <c r="DG2">
+        <v>1</v>
+      </c>
+      <c r="DH2">
+        <v>1</v>
+      </c>
+      <c r="DI2">
+        <v>1</v>
+      </c>
+      <c r="DJ2">
+        <v>1</v>
+      </c>
+      <c r="DK2">
+        <v>1</v>
+      </c>
+      <c r="DL2">
+        <v>1</v>
+      </c>
+      <c r="DM2">
+        <v>1</v>
+      </c>
+      <c r="DN2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:109">
+    <row r="3" spans="1:118">
       <c r="A3" s="1" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -3641,129 +3881,156 @@
         <v>0</v>
       </c>
       <c r="BR3">
-        <v>0.01081915549833977</v>
+        <v>0</v>
       </c>
       <c r="BS3">
-        <v>0.04232461172594491</v>
+        <v>0</v>
       </c>
       <c r="BT3">
-        <v>0.04326590852874307</v>
+        <v>0</v>
       </c>
       <c r="BU3">
-        <v>0.07283887776162462</v>
+        <v>0</v>
       </c>
       <c r="BV3">
-        <v>0.07649154052737477</v>
+        <v>0</v>
       </c>
       <c r="BW3">
-        <v>0.09915164587840766</v>
+        <v>0</v>
       </c>
       <c r="BX3">
-        <v>0.1096427376512802</v>
+        <v>0</v>
       </c>
       <c r="BY3">
-        <v>0.1135039816620311</v>
+        <v>0</v>
       </c>
       <c r="BZ3">
-        <v>0.1185913051849197</v>
+        <v>0</v>
       </c>
       <c r="CA3">
-        <v>0.1738260216127834</v>
+        <v>0</v>
       </c>
       <c r="CB3">
-        <v>0.2717797571312274</v>
+        <v>0</v>
       </c>
       <c r="CC3">
-        <v>0.3080061926054702</v>
+        <v>0</v>
       </c>
       <c r="CD3">
-        <v>0.3095112563260986</v>
+        <v>0</v>
       </c>
       <c r="CE3">
-        <v>0.3530108525713396</v>
+        <v>0</v>
       </c>
       <c r="CF3">
-        <v>0.4526190186511205</v>
+        <v>0</v>
       </c>
       <c r="CG3">
-        <v>0.5297651908363886</v>
+        <v>0</v>
       </c>
       <c r="CH3">
-        <v>0.542626331190832</v>
+        <v>0</v>
       </c>
       <c r="CI3">
-        <v>0.5463728677025583</v>
+        <v>0.04910644800970281</v>
       </c>
       <c r="CJ3">
-        <v>0.5677627766565008</v>
+        <v>0.05488388478819618</v>
       </c>
       <c r="CK3">
-        <v>0.6042279348164199</v>
+        <v>0.266580023333093</v>
       </c>
       <c r="CL3">
-        <v>0.6540101554433017</v>
+        <v>0.3406043466357271</v>
       </c>
       <c r="CM3">
-        <v>0.6971396750348304</v>
+        <v>0.3445622027139666</v>
       </c>
       <c r="CN3">
-        <v>0.7246249943637788</v>
+        <v>0.3478713505478269</v>
       </c>
       <c r="CO3">
-        <v>0.7517472246412154</v>
+        <v>0.4644601852873658</v>
       </c>
       <c r="CP3">
-        <v>0.7644626162792385</v>
+        <v>0.6810760767062916</v>
       </c>
       <c r="CQ3">
-        <v>0.7684341910025483</v>
+        <v>0.681125813911829</v>
       </c>
       <c r="CR3">
-        <v>0.8125006393850915</v>
+        <v>0.7154513017890143</v>
       </c>
       <c r="CS3">
-        <v>0.8689993849854466</v>
+        <v>0.7335132779524781</v>
       </c>
       <c r="CT3">
-        <v>0.9180092009106083</v>
+        <v>0.7349584281504425</v>
       </c>
       <c r="CU3">
-        <v>0.9587418961869443</v>
+        <v>0.7614126515249763</v>
       </c>
       <c r="CV3">
-        <v>0.9885825627869227</v>
+        <v>0.7663987191525743</v>
       </c>
       <c r="CW3">
-        <v>1</v>
+        <v>0.7842877014869475</v>
       </c>
       <c r="CX3">
-        <v>1</v>
+        <v>0.8402445083605282</v>
       </c>
       <c r="CY3">
-        <v>1</v>
+        <v>0.8549046388834187</v>
       </c>
       <c r="CZ3">
-        <v>1</v>
+        <v>0.8619784249072595</v>
       </c>
       <c r="DA3">
-        <v>1</v>
+        <v>0.8625060337237372</v>
       </c>
       <c r="DB3">
-        <v>1</v>
+        <v>0.865963241512806</v>
       </c>
       <c r="DC3">
-        <v>1</v>
+        <v>0.8861690867602757</v>
       </c>
       <c r="DD3">
-        <v>1</v>
+        <v>0.9241682543077406</v>
       </c>
       <c r="DE3">
+        <v>0.9276524204462511</v>
+      </c>
+      <c r="DF3">
+        <v>0.9346441890487124</v>
+      </c>
+      <c r="DG3">
+        <v>0.9400192623159324</v>
+      </c>
+      <c r="DH3">
+        <v>0.940697923997693</v>
+      </c>
+      <c r="DI3">
+        <v>0.957832562679179</v>
+      </c>
+      <c r="DJ3">
+        <v>0.9582572137210427</v>
+      </c>
+      <c r="DK3">
+        <v>0.9717018881585212</v>
+      </c>
+      <c r="DL3">
+        <v>0.9787079823739882</v>
+      </c>
+      <c r="DM3">
+        <v>0.9950461513620572</v>
+      </c>
+      <c r="DN3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:109">
+    <row r="4" spans="1:118">
       <c r="A4" s="1" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -3994,105 +4261,132 @@
         <v>0</v>
       </c>
       <c r="BZ4">
-        <v>0.01407148980537029</v>
+        <v>0</v>
       </c>
       <c r="CA4">
-        <v>0.07943252602458423</v>
+        <v>0</v>
       </c>
       <c r="CB4">
-        <v>0.09168172407932981</v>
+        <v>0</v>
       </c>
       <c r="CC4">
-        <v>0.151116042955673</v>
+        <v>0</v>
       </c>
       <c r="CD4">
-        <v>0.1538621537975915</v>
+        <v>0</v>
       </c>
       <c r="CE4">
-        <v>0.2040419898181906</v>
+        <v>0</v>
       </c>
       <c r="CF4">
-        <v>0.2318001419552312</v>
+        <v>0</v>
       </c>
       <c r="CG4">
-        <v>0.2414857946959879</v>
+        <v>0.05918418727449985</v>
       </c>
       <c r="CH4">
-        <v>0.2427510614113632</v>
+        <v>0.09059134324048229</v>
       </c>
       <c r="CI4">
-        <v>0.3136768884616924</v>
+        <v>0.1790838837984702</v>
       </c>
       <c r="CJ4">
-        <v>0.3943117035653396</v>
+        <v>0.2032773592672625</v>
       </c>
       <c r="CK4">
-        <v>0.4149953372675271</v>
+        <v>0.203300803434311</v>
       </c>
       <c r="CL4">
-        <v>0.4215603538979734</v>
+        <v>0.2475893697582831</v>
       </c>
       <c r="CM4">
-        <v>0.4817562386019802</v>
+        <v>0.3383646806798751</v>
       </c>
       <c r="CN4">
-        <v>0.5752476257762934</v>
+        <v>0.4066089258050708</v>
       </c>
       <c r="CO4">
-        <v>0.6285684455504381</v>
+        <v>0.4113885439405996</v>
       </c>
       <c r="CP4">
-        <v>0.6324136583794092</v>
+        <v>0.420231033980421</v>
       </c>
       <c r="CQ4">
-        <v>0.637752390123936</v>
+        <v>0.421256631826491</v>
       </c>
       <c r="CR4">
-        <v>0.6596317976135988</v>
+        <v>0.5963009204833427</v>
       </c>
       <c r="CS4">
-        <v>0.6936663878724645</v>
+        <v>0.5988714435808353</v>
       </c>
       <c r="CT4">
-        <v>0.7376952668672165</v>
+        <v>0.6214229785935178</v>
       </c>
       <c r="CU4">
-        <v>0.7806549069301678</v>
+        <v>0.6964496713664138</v>
       </c>
       <c r="CV4">
-        <v>0.806251151218155</v>
+        <v>0.7869069012236943</v>
       </c>
       <c r="CW4">
-        <v>0.8202295286103227</v>
+        <v>0.8095602792439999</v>
       </c>
       <c r="CX4">
-        <v>0.8224279585017573</v>
+        <v>0.8097788459428118</v>
       </c>
       <c r="CY4">
-        <v>0.8293592133090851</v>
+        <v>0.8382153447150461</v>
       </c>
       <c r="CZ4">
-        <v>0.8660408992818394</v>
+        <v>0.9440372309802383</v>
       </c>
       <c r="DA4">
-        <v>0.9156439749591484</v>
+        <v>0.9668499621951029</v>
       </c>
       <c r="DB4">
-        <v>0.9537695799111348</v>
+        <v>0.9674973011149099</v>
       </c>
       <c r="DC4">
-        <v>0.9789021185761844</v>
+        <v>0.9691297796400578</v>
       </c>
       <c r="DD4">
-        <v>0.9953427413084648</v>
+        <v>0.9711606261339604</v>
       </c>
       <c r="DE4">
-        <v>1</v>
+        <v>0.9795921719137841</v>
+      </c>
+      <c r="DF4">
+        <v>0.9824745806823766</v>
+      </c>
+      <c r="DG4">
+        <v>0.982677890613005</v>
+      </c>
+      <c r="DH4">
+        <v>0.9830204165068464</v>
+      </c>
+      <c r="DI4">
+        <v>0.983064225784433</v>
+      </c>
+      <c r="DJ4">
+        <v>0.9912561086925991</v>
+      </c>
+      <c r="DK4">
+        <v>0.9917294101172905</v>
+      </c>
+      <c r="DL4">
+        <v>0.9999999999999997</v>
+      </c>
+      <c r="DM4">
+        <v>0.9999999999999997</v>
+      </c>
+      <c r="DN4">
+        <v>0.9999999999999997</v>
       </c>
     </row>
-    <row r="5" spans="1:109">
+    <row r="5" spans="1:118">
       <c r="A5" s="1" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -4206,222 +4500,249 @@
         <v>0</v>
       </c>
       <c r="AM5">
-        <v>0.04942376589392553</v>
+        <v>0</v>
       </c>
       <c r="AN5">
-        <v>0.06788008119124686</v>
+        <v>0</v>
       </c>
       <c r="AO5">
-        <v>0.06788008119124686</v>
+        <v>0</v>
       </c>
       <c r="AP5">
-        <v>0.07421607345057858</v>
+        <v>0</v>
       </c>
       <c r="AQ5">
-        <v>0.07806100054527471</v>
+        <v>0</v>
       </c>
       <c r="AR5">
-        <v>0.07812995856132042</v>
+        <v>0</v>
       </c>
       <c r="AS5">
-        <v>0.0805819908405712</v>
+        <v>0</v>
       </c>
       <c r="AT5">
-        <v>0.1036209537276516</v>
+        <v>0</v>
       </c>
       <c r="AU5">
-        <v>0.1742186337533963</v>
+        <v>0</v>
       </c>
       <c r="AV5">
-        <v>0.2626147404645181</v>
+        <v>0</v>
       </c>
       <c r="AW5">
-        <v>0.3560970124491007</v>
+        <v>0</v>
       </c>
       <c r="AX5">
-        <v>0.41850152589971</v>
+        <v>0</v>
       </c>
       <c r="AY5">
-        <v>0.4620950904651929</v>
+        <v>0</v>
       </c>
       <c r="AZ5">
-        <v>0.4809603580740354</v>
+        <v>0</v>
       </c>
       <c r="BA5">
-        <v>0.5032361940290015</v>
+        <v>0</v>
       </c>
       <c r="BB5">
-        <v>0.5248464725360273</v>
+        <v>0</v>
       </c>
       <c r="BC5">
-        <v>0.5265997810544217</v>
+        <v>0</v>
       </c>
       <c r="BD5">
-        <v>0.5265997810544217</v>
+        <v>0</v>
       </c>
       <c r="BE5">
-        <v>0.5291041927248867</v>
+        <v>0</v>
       </c>
       <c r="BF5">
-        <v>0.5294526592781066</v>
+        <v>0</v>
       </c>
       <c r="BG5">
-        <v>0.5294526592781066</v>
+        <v>0</v>
       </c>
       <c r="BH5">
-        <v>0.5348964048168179</v>
+        <v>0</v>
       </c>
       <c r="BI5">
-        <v>0.5857658369794767</v>
+        <v>0</v>
       </c>
       <c r="BJ5">
-        <v>0.6701035584507844</v>
+        <v>0</v>
       </c>
       <c r="BK5">
-        <v>0.7541922940283627</v>
+        <v>0</v>
       </c>
       <c r="BL5">
-        <v>0.784718287108837</v>
+        <v>0</v>
       </c>
       <c r="BM5">
-        <v>0.7996391607620412</v>
+        <v>0</v>
       </c>
       <c r="BN5">
-        <v>0.8283773670798554</v>
+        <v>0</v>
       </c>
       <c r="BO5">
-        <v>0.8962038342407759</v>
+        <v>0</v>
       </c>
       <c r="BP5">
-        <v>0.9580873654243998</v>
+        <v>0</v>
       </c>
       <c r="BQ5">
-        <v>0.9580873654243998</v>
+        <v>0</v>
       </c>
       <c r="BR5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BS5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BT5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BU5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BV5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BW5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BY5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BZ5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CA5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CB5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CC5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CD5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CE5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CF5">
-        <v>1</v>
+        <v>0.03059814523646267</v>
       </c>
       <c r="CG5">
-        <v>1</v>
+        <v>0.04751092016852211</v>
       </c>
       <c r="CH5">
-        <v>1</v>
+        <v>0.08827523430617099</v>
       </c>
       <c r="CI5">
-        <v>1</v>
+        <v>0.09737010203469575</v>
       </c>
       <c r="CJ5">
-        <v>1</v>
+        <v>0.1044148847251801</v>
       </c>
       <c r="CK5">
-        <v>1</v>
+        <v>0.1103224465183198</v>
       </c>
       <c r="CL5">
-        <v>1</v>
+        <v>0.1467845770728351</v>
       </c>
       <c r="CM5">
-        <v>1</v>
+        <v>0.2345953093281994</v>
       </c>
       <c r="CN5">
-        <v>1</v>
+        <v>0.2347573197447288</v>
       </c>
       <c r="CO5">
-        <v>1</v>
+        <v>0.2652280015071442</v>
       </c>
       <c r="CP5">
-        <v>1</v>
+        <v>0.2918405397046965</v>
       </c>
       <c r="CQ5">
-        <v>1</v>
+        <v>0.391122705716849</v>
       </c>
       <c r="CR5">
-        <v>1</v>
+        <v>0.5022040880349891</v>
       </c>
       <c r="CS5">
-        <v>1</v>
+        <v>0.5165302276175637</v>
       </c>
       <c r="CT5">
-        <v>1</v>
+        <v>0.5165302276175637</v>
       </c>
       <c r="CU5">
-        <v>1</v>
+        <v>0.6250571212952202</v>
       </c>
       <c r="CV5">
-        <v>1</v>
+        <v>0.6979393589743089</v>
       </c>
       <c r="CW5">
-        <v>1</v>
+        <v>0.6981727891983927</v>
       </c>
       <c r="CX5">
-        <v>1</v>
+        <v>0.6981727891983927</v>
       </c>
       <c r="CY5">
-        <v>1</v>
+        <v>0.817221508504411</v>
       </c>
       <c r="CZ5">
-        <v>1</v>
+        <v>0.9464319203848373</v>
       </c>
       <c r="DA5">
-        <v>1</v>
+        <v>0.9474989012256</v>
       </c>
       <c r="DB5">
-        <v>1</v>
+        <v>0.9539198201031773</v>
       </c>
       <c r="DC5">
-        <v>1</v>
+        <v>0.955209748168524</v>
       </c>
       <c r="DD5">
-        <v>1</v>
+        <v>0.958121560712473</v>
       </c>
       <c r="DE5">
+        <v>0.9593987955332921</v>
+      </c>
+      <c r="DF5">
+        <v>0.9689415298353105</v>
+      </c>
+      <c r="DG5">
+        <v>0.9710116654483362</v>
+      </c>
+      <c r="DH5">
+        <v>0.9718088151058548</v>
+      </c>
+      <c r="DI5">
+        <v>0.9950495939855732</v>
+      </c>
+      <c r="DJ5">
+        <v>0.9995076032535691</v>
+      </c>
+      <c r="DK5">
+        <v>1</v>
+      </c>
+      <c r="DL5">
+        <v>1</v>
+      </c>
+      <c r="DM5">
+        <v>1</v>
+      </c>
+      <c r="DN5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:109">
+    <row r="6" spans="1:118">
       <c r="A6" s="1" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -4430,321 +4751,348 @@
         <v>0</v>
       </c>
       <c r="D6">
-        <v>0.004111641918218757</v>
+        <v>0</v>
       </c>
       <c r="E6">
-        <v>0.004237079321138074</v>
+        <v>0</v>
       </c>
       <c r="F6">
-        <v>0.01114331047208044</v>
+        <v>0</v>
       </c>
       <c r="G6">
-        <v>0.01114427151872446</v>
+        <v>0</v>
       </c>
       <c r="H6">
-        <v>0.01369770395562653</v>
+        <v>0</v>
       </c>
       <c r="I6">
-        <v>0.01800967471816458</v>
+        <v>0</v>
       </c>
       <c r="J6">
-        <v>0.01865197770570929</v>
+        <v>0</v>
       </c>
       <c r="K6">
-        <v>0.01979291803541204</v>
+        <v>0</v>
       </c>
       <c r="L6">
-        <v>0.02615950307757887</v>
+        <v>0</v>
       </c>
       <c r="M6">
-        <v>0.04325360519049124</v>
+        <v>0</v>
       </c>
       <c r="N6">
-        <v>0.05059832000682812</v>
+        <v>0</v>
       </c>
       <c r="O6">
-        <v>0.05059930591766807</v>
+        <v>0</v>
       </c>
       <c r="P6">
-        <v>0.05787828770475059</v>
+        <v>0</v>
       </c>
       <c r="Q6">
-        <v>0.07500972006305309</v>
+        <v>0</v>
       </c>
       <c r="R6">
-        <v>0.09183213786740775</v>
+        <v>0</v>
       </c>
       <c r="S6">
-        <v>0.09576472430754322</v>
+        <v>0</v>
       </c>
       <c r="T6">
-        <v>0.09584610078666149</v>
+        <v>0</v>
       </c>
       <c r="U6">
-        <v>0.09846158094694596</v>
+        <v>0</v>
       </c>
       <c r="V6">
-        <v>0.1038505863365428</v>
+        <v>0</v>
       </c>
       <c r="W6">
-        <v>0.1135938494214635</v>
+        <v>0</v>
       </c>
       <c r="X6">
-        <v>0.1589466476395717</v>
+        <v>0</v>
       </c>
       <c r="Y6">
-        <v>0.2484153365877717</v>
+        <v>0</v>
       </c>
       <c r="Z6">
-        <v>0.3179869244580683</v>
+        <v>0</v>
       </c>
       <c r="AA6">
-        <v>0.3492131710279299</v>
+        <v>0</v>
       </c>
       <c r="AB6">
-        <v>0.3520962040439786</v>
+        <v>0</v>
       </c>
       <c r="AC6">
-        <v>0.4459592733795346</v>
+        <v>0</v>
       </c>
       <c r="AD6">
-        <v>0.6061807974707327</v>
+        <v>0</v>
       </c>
       <c r="AE6">
-        <v>0.7487876371216838</v>
+        <v>0</v>
       </c>
       <c r="AF6">
-        <v>0.8595670248128249</v>
+        <v>0</v>
       </c>
       <c r="AG6">
-        <v>0.9522229871418926</v>
+        <v>0</v>
       </c>
       <c r="AH6">
-        <v>0.9932475156804488</v>
+        <v>0</v>
       </c>
       <c r="AI6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AP6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AQ6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AS6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AT6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AU6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AV6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AX6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AY6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AZ6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BC6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BD6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BE6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BF6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BG6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BH6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BI6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BJ6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BK6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BL6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BM6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BN6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BO6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BP6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BQ6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BR6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BS6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BT6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BU6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BV6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BW6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BY6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BZ6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CA6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CB6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CC6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CD6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CE6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CF6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CG6">
-        <v>1</v>
+        <v>0.05794142923749691</v>
       </c>
       <c r="CH6">
-        <v>1</v>
+        <v>0.0653594548183937</v>
       </c>
       <c r="CI6">
-        <v>1</v>
+        <v>0.1647425537392248</v>
       </c>
       <c r="CJ6">
-        <v>1</v>
+        <v>0.2487959905256251</v>
       </c>
       <c r="CK6">
-        <v>1</v>
+        <v>0.2524093812915696</v>
       </c>
       <c r="CL6">
-        <v>1</v>
+        <v>0.2907859947085869</v>
       </c>
       <c r="CM6">
-        <v>1</v>
+        <v>0.3470456100066266</v>
       </c>
       <c r="CN6">
-        <v>1</v>
+        <v>0.406389922512461</v>
       </c>
       <c r="CO6">
-        <v>1</v>
+        <v>0.4281608894026567</v>
       </c>
       <c r="CP6">
-        <v>1</v>
+        <v>0.4406989731587392</v>
       </c>
       <c r="CQ6">
-        <v>1</v>
+        <v>0.4407076096041095</v>
       </c>
       <c r="CR6">
-        <v>1</v>
+        <v>0.5964433585464042</v>
       </c>
       <c r="CS6">
-        <v>1</v>
+        <v>0.6041444960248475</v>
       </c>
       <c r="CT6">
-        <v>1</v>
+        <v>0.6414239278768514</v>
       </c>
       <c r="CU6">
-        <v>1</v>
+        <v>0.6444743926114286</v>
       </c>
       <c r="CV6">
-        <v>1</v>
+        <v>0.7422143565259257</v>
       </c>
       <c r="CW6">
-        <v>1</v>
+        <v>0.8244363436544547</v>
       </c>
       <c r="CX6">
-        <v>1</v>
+        <v>0.8244473869775676</v>
       </c>
       <c r="CY6">
-        <v>1</v>
+        <v>0.8863629590676718</v>
       </c>
       <c r="CZ6">
-        <v>1</v>
+        <v>0.9664030314822475</v>
       </c>
       <c r="DA6">
-        <v>1</v>
+        <v>0.9664147275302187</v>
       </c>
       <c r="DB6">
-        <v>1</v>
+        <v>0.9672568787285567</v>
       </c>
       <c r="DC6">
-        <v>1</v>
+        <v>0.9675352811113472</v>
       </c>
       <c r="DD6">
-        <v>1</v>
+        <v>0.9724352244799743</v>
       </c>
       <c r="DE6">
+        <v>0.9737566791071146</v>
+      </c>
+      <c r="DF6">
+        <v>0.9796337937301692</v>
+      </c>
+      <c r="DG6">
+        <v>0.9824024021776914</v>
+      </c>
+      <c r="DH6">
+        <v>0.9828451322677588</v>
+      </c>
+      <c r="DI6">
+        <v>0.9829260683111947</v>
+      </c>
+      <c r="DJ6">
+        <v>0.9906160467403666</v>
+      </c>
+      <c r="DK6">
+        <v>0.990669367135576</v>
+      </c>
+      <c r="DL6">
+        <v>1</v>
+      </c>
+      <c r="DM6">
+        <v>1</v>
+      </c>
+      <c r="DN6">
         <v>1</v>
       </c>
     </row>
@@ -4763,302 +5111,287 @@
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" s="1" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>120</v>
+        <v>129</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>128</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:16">
       <c r="A2" s="1" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="B2">
         <v>0.5</v>
       </c>
       <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2">
         <v>11</v>
       </c>
-      <c r="D2">
-        <v>29</v>
-      </c>
       <c r="E2">
-        <v>0.01017582932584769</v>
+        <v>0.1233766198757316</v>
       </c>
       <c r="F2">
-        <v>0.5140446220816962</v>
+        <v>0.5225208583041787</v>
       </c>
       <c r="G2">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="H2">
         <v>600</v>
       </c>
       <c r="I2" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="J2" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="K2" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="L2">
-        <v>323</v>
+        <v>139</v>
       </c>
       <c r="M2">
         <v>600</v>
       </c>
       <c r="N2" t="s">
-        <v>132</v>
-      </c>
-      <c r="O2" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="P2" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:16">
       <c r="A3" s="1" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="B3">
         <v>0.5</v>
       </c>
       <c r="C3">
-        <v>69</v>
+        <v>88</v>
       </c>
       <c r="D3">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="E3">
-        <v>0.01081915549833977</v>
+        <v>0.266580023333093</v>
       </c>
       <c r="F3">
-        <v>0.5297651908363886</v>
+        <v>0.6810760767062916</v>
       </c>
       <c r="G3">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="H3">
         <v>600</v>
       </c>
       <c r="I3" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="J3" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="K3" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="L3">
-        <v>323</v>
+        <v>139</v>
       </c>
       <c r="M3">
         <v>600</v>
       </c>
       <c r="N3" t="s">
-        <v>132</v>
-      </c>
-      <c r="O3" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="P3" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:16">
       <c r="A4" s="1" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="B4">
         <v>0.5</v>
       </c>
       <c r="C4">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D4">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="E4">
-        <v>0.01407148980537029</v>
+        <v>0.09059134324048229</v>
       </c>
       <c r="F4">
-        <v>0.5752476257762934</v>
+        <v>0.5963009204833427</v>
       </c>
       <c r="G4">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="H4">
         <v>600</v>
       </c>
       <c r="I4" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="J4" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="K4" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="L4">
-        <v>323</v>
+        <v>139</v>
       </c>
       <c r="M4">
         <v>600</v>
       </c>
       <c r="N4" t="s">
-        <v>132</v>
-      </c>
-      <c r="O4" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="P4" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
     </row>
     <row r="5" spans="1:16">
       <c r="A5" s="1" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="B5">
         <v>0.5</v>
       </c>
       <c r="C5">
-        <v>38</v>
+        <v>85</v>
       </c>
       <c r="D5">
-        <v>52</v>
+        <v>95</v>
       </c>
       <c r="E5">
-        <v>0.04942376589392553</v>
+        <v>0.08827523430617099</v>
       </c>
       <c r="F5">
-        <v>0.5032361940290015</v>
+        <v>0.5022040880349891</v>
       </c>
       <c r="G5">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="H5">
         <v>600</v>
       </c>
       <c r="I5" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="J5" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="K5" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="L5">
-        <v>323</v>
+        <v>139</v>
       </c>
       <c r="M5">
         <v>600</v>
       </c>
       <c r="N5" t="s">
-        <v>132</v>
-      </c>
-      <c r="O5" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="P5" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:16">
       <c r="A6" s="1" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="B6">
         <v>0.5</v>
       </c>
       <c r="C6">
-        <v>5</v>
+        <v>86</v>
       </c>
       <c r="D6">
-        <v>29</v>
+        <v>95</v>
       </c>
       <c r="E6">
-        <v>0.01114331047208044</v>
+        <v>0.1647425537392248</v>
       </c>
       <c r="F6">
-        <v>0.6061807974707327</v>
+        <v>0.5964433585464042</v>
       </c>
       <c r="G6">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="H6">
         <v>600</v>
       </c>
       <c r="I6" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="J6" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="K6" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="L6">
-        <v>323</v>
+        <v>139</v>
       </c>
       <c r="M6">
         <v>600</v>
       </c>
       <c r="N6" t="s">
-        <v>132</v>
-      </c>
-      <c r="O6" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="P6" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -5076,302 +5409,287 @@
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" s="1" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>120</v>
+        <v>129</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>128</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:16">
       <c r="A2" s="1" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="B2">
         <v>0.7</v>
       </c>
       <c r="C2">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D2">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="E2">
-        <v>0.01017582932584769</v>
+        <v>0.1233766198757316</v>
       </c>
       <c r="F2">
-        <v>0.7623171864649519</v>
+        <v>0.7692198782434589</v>
       </c>
       <c r="G2">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="H2">
         <v>600</v>
       </c>
       <c r="I2" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="J2" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="K2" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="L2">
-        <v>323</v>
+        <v>139</v>
       </c>
       <c r="M2">
         <v>600</v>
       </c>
       <c r="N2" t="s">
-        <v>132</v>
-      </c>
-      <c r="O2" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="P2" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:16">
       <c r="A3" s="1" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="B3">
         <v>0.7</v>
       </c>
       <c r="C3">
-        <v>69</v>
+        <v>88</v>
       </c>
       <c r="D3">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="E3">
-        <v>0.01081915549833977</v>
+        <v>0.266580023333093</v>
       </c>
       <c r="F3">
-        <v>0.7246249943637788</v>
+        <v>0.7154513017890143</v>
       </c>
       <c r="G3">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="H3">
         <v>600</v>
       </c>
       <c r="I3" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="J3" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="K3" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="L3">
-        <v>323</v>
+        <v>139</v>
       </c>
       <c r="M3">
         <v>600</v>
       </c>
       <c r="N3" t="s">
-        <v>132</v>
-      </c>
-      <c r="O3" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="P3" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:16">
       <c r="A4" s="1" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="B4">
         <v>0.7</v>
       </c>
       <c r="C4">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D4">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E4">
-        <v>0.01407148980537029</v>
+        <v>0.09059134324048229</v>
       </c>
       <c r="F4">
-        <v>0.7376952668672165</v>
+        <v>0.7869069012236943</v>
       </c>
       <c r="G4">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="H4">
         <v>600</v>
       </c>
       <c r="I4" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="J4" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="K4" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="L4">
-        <v>323</v>
+        <v>139</v>
       </c>
       <c r="M4">
         <v>600</v>
       </c>
       <c r="N4" t="s">
-        <v>132</v>
-      </c>
-      <c r="O4" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="P4" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
     </row>
     <row r="5" spans="1:16">
       <c r="A5" s="1" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="B5">
         <v>0.7</v>
       </c>
       <c r="C5">
-        <v>38</v>
+        <v>85</v>
       </c>
       <c r="D5">
-        <v>62</v>
+        <v>102</v>
       </c>
       <c r="E5">
-        <v>0.04942376589392553</v>
+        <v>0.08827523430617099</v>
       </c>
       <c r="F5">
-        <v>0.7541922940283627</v>
+        <v>0.817221508504411</v>
       </c>
       <c r="G5">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="H5">
         <v>600</v>
       </c>
       <c r="I5" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="J5" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="K5" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="L5">
-        <v>323</v>
+        <v>139</v>
       </c>
       <c r="M5">
         <v>600</v>
       </c>
       <c r="N5" t="s">
-        <v>132</v>
-      </c>
-      <c r="O5" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="P5" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:16">
       <c r="A6" s="1" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="B6">
         <v>0.7</v>
       </c>
       <c r="C6">
-        <v>5</v>
+        <v>86</v>
       </c>
       <c r="D6">
-        <v>30</v>
+        <v>99</v>
       </c>
       <c r="E6">
-        <v>0.01114331047208044</v>
+        <v>0.1647425537392248</v>
       </c>
       <c r="F6">
-        <v>0.7487876371216838</v>
+        <v>0.7422143565259257</v>
       </c>
       <c r="G6">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="H6">
         <v>600</v>
       </c>
       <c r="I6" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="J6" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="K6" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="L6">
-        <v>323</v>
+        <v>139</v>
       </c>
       <c r="M6">
         <v>600</v>
       </c>
       <c r="N6" t="s">
-        <v>132</v>
-      </c>
-      <c r="O6" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="P6" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -5389,302 +5707,287 @@
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" s="1" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>120</v>
+        <v>129</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>128</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:16">
       <c r="A2" s="1" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="B2">
         <v>0.8</v>
       </c>
       <c r="C2">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D2">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="E2">
-        <v>0.01017582932584769</v>
+        <v>0.1233766198757316</v>
       </c>
       <c r="F2">
-        <v>0.8857371739936715</v>
+        <v>0.8119305829755058</v>
       </c>
       <c r="G2">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="H2">
         <v>600</v>
       </c>
       <c r="I2" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="J2" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="K2" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="L2">
-        <v>323</v>
+        <v>139</v>
       </c>
       <c r="M2">
         <v>600</v>
       </c>
       <c r="N2" t="s">
-        <v>132</v>
-      </c>
-      <c r="O2" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="P2" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:16">
       <c r="A3" s="1" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="B3">
         <v>0.8</v>
       </c>
       <c r="C3">
-        <v>69</v>
+        <v>88</v>
       </c>
       <c r="D3">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="E3">
-        <v>0.01081915549833977</v>
+        <v>0.266580023333093</v>
       </c>
       <c r="F3">
-        <v>0.8125006393850915</v>
+        <v>0.8402445083605282</v>
       </c>
       <c r="G3">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="H3">
         <v>600</v>
       </c>
       <c r="I3" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="J3" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="K3" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="L3">
-        <v>323</v>
+        <v>139</v>
       </c>
       <c r="M3">
         <v>600</v>
       </c>
       <c r="N3" t="s">
-        <v>132</v>
-      </c>
-      <c r="O3" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="P3" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:16">
       <c r="A4" s="1" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="B4">
         <v>0.8</v>
       </c>
       <c r="C4">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D4">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E4">
-        <v>0.01407148980537029</v>
+        <v>0.09059134324048229</v>
       </c>
       <c r="F4">
-        <v>0.806251151218155</v>
+        <v>0.8095602792439999</v>
       </c>
       <c r="G4">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="H4">
         <v>600</v>
       </c>
       <c r="I4" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="J4" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="K4" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="L4">
-        <v>323</v>
+        <v>139</v>
       </c>
       <c r="M4">
         <v>600</v>
       </c>
       <c r="N4" t="s">
-        <v>132</v>
-      </c>
-      <c r="O4" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="P4" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
     </row>
     <row r="5" spans="1:16">
       <c r="A5" s="1" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="B5">
         <v>0.8</v>
       </c>
       <c r="C5">
-        <v>38</v>
+        <v>85</v>
       </c>
       <c r="D5">
-        <v>65</v>
+        <v>102</v>
       </c>
       <c r="E5">
-        <v>0.04942376589392553</v>
+        <v>0.08827523430617099</v>
       </c>
       <c r="F5">
-        <v>0.8283773670798554</v>
+        <v>0.817221508504411</v>
       </c>
       <c r="G5">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="H5">
         <v>600</v>
       </c>
       <c r="I5" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="J5" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="K5" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="L5">
-        <v>323</v>
+        <v>139</v>
       </c>
       <c r="M5">
         <v>600</v>
       </c>
       <c r="N5" t="s">
-        <v>132</v>
-      </c>
-      <c r="O5" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="P5" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:16">
       <c r="A6" s="1" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="B6">
         <v>0.8</v>
       </c>
       <c r="C6">
-        <v>5</v>
+        <v>86</v>
       </c>
       <c r="D6">
-        <v>31</v>
+        <v>100</v>
       </c>
       <c r="E6">
-        <v>0.01114331047208044</v>
+        <v>0.1647425537392248</v>
       </c>
       <c r="F6">
-        <v>0.8595670248128249</v>
+        <v>0.8244363436544547</v>
       </c>
       <c r="G6">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="H6">
         <v>600</v>
       </c>
       <c r="I6" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="J6" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="K6" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="L6">
-        <v>323</v>
+        <v>139</v>
       </c>
       <c r="M6">
         <v>600</v>
       </c>
       <c r="N6" t="s">
-        <v>132</v>
-      </c>
-      <c r="O6" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="P6" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -5702,302 +6005,287 @@
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" s="1" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>120</v>
+        <v>129</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>128</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:16">
       <c r="A2" s="1" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="B2">
         <v>0.9</v>
       </c>
       <c r="C2">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D2">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="E2">
-        <v>0.01017582932584769</v>
+        <v>0.1233766198757316</v>
       </c>
       <c r="F2">
-        <v>0.9709582403828004</v>
+        <v>0.922723577108264</v>
       </c>
       <c r="G2">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="H2">
         <v>600</v>
       </c>
       <c r="I2" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="J2" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="K2" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="L2">
-        <v>323</v>
+        <v>139</v>
       </c>
       <c r="M2">
         <v>600</v>
       </c>
       <c r="N2" t="s">
-        <v>132</v>
-      </c>
-      <c r="O2" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="P2" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:16">
       <c r="A3" s="1" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="B3">
         <v>0.9</v>
       </c>
       <c r="C3">
-        <v>69</v>
+        <v>88</v>
       </c>
       <c r="D3">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="E3">
-        <v>0.01081915549833977</v>
+        <v>0.266580023333093</v>
       </c>
       <c r="F3">
-        <v>0.9180092009106083</v>
+        <v>0.9241682543077406</v>
       </c>
       <c r="G3">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="H3">
         <v>600</v>
       </c>
       <c r="I3" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="J3" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="K3" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="L3">
-        <v>323</v>
+        <v>139</v>
       </c>
       <c r="M3">
         <v>600</v>
       </c>
       <c r="N3" t="s">
-        <v>132</v>
-      </c>
-      <c r="O3" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="P3" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:16">
       <c r="A4" s="1" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="B4">
         <v>0.9</v>
       </c>
       <c r="C4">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D4">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E4">
-        <v>0.01407148980537029</v>
+        <v>0.09059134324048229</v>
       </c>
       <c r="F4">
-        <v>0.9156439749591484</v>
+        <v>0.9440372309802383</v>
       </c>
       <c r="G4">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="H4">
         <v>600</v>
       </c>
       <c r="I4" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="J4" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="K4" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="L4">
-        <v>323</v>
+        <v>139</v>
       </c>
       <c r="M4">
         <v>600</v>
       </c>
       <c r="N4" t="s">
-        <v>132</v>
-      </c>
-      <c r="O4" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="P4" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
     </row>
     <row r="5" spans="1:16">
       <c r="A5" s="1" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="B5">
         <v>0.9</v>
       </c>
       <c r="C5">
-        <v>38</v>
+        <v>85</v>
       </c>
       <c r="D5">
-        <v>67</v>
+        <v>103</v>
       </c>
       <c r="E5">
-        <v>0.04942376589392553</v>
+        <v>0.08827523430617099</v>
       </c>
       <c r="F5">
-        <v>0.9580873654243998</v>
+        <v>0.9464319203848373</v>
       </c>
       <c r="G5">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="H5">
         <v>600</v>
       </c>
       <c r="I5" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="J5" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="K5" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="L5">
-        <v>323</v>
+        <v>139</v>
       </c>
       <c r="M5">
         <v>600</v>
       </c>
       <c r="N5" t="s">
-        <v>132</v>
-      </c>
-      <c r="O5" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="P5" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:16">
       <c r="A6" s="1" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="B6">
         <v>0.9</v>
       </c>
       <c r="C6">
-        <v>5</v>
+        <v>86</v>
       </c>
       <c r="D6">
-        <v>32</v>
+        <v>103</v>
       </c>
       <c r="E6">
-        <v>0.01114331047208044</v>
+        <v>0.1647425537392248</v>
       </c>
       <c r="F6">
-        <v>0.9522229871418926</v>
+        <v>0.9664030314822475</v>
       </c>
       <c r="G6">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="H6">
         <v>600</v>
       </c>
       <c r="I6" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="J6" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="K6" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="L6">
-        <v>323</v>
+        <v>139</v>
       </c>
       <c r="M6">
         <v>600</v>
       </c>
       <c r="N6" t="s">
-        <v>132</v>
-      </c>
-      <c r="O6" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="P6" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>